<commit_message>
weeklyreport : instruction + couleur
</commit_message>
<xml_diff>
--- a/lib/PHPExcel/templates/WeeklyReport.xlsx
+++ b/lib/PHPExcel/templates/WeeklyReport.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\GPM\lib\PHPExcel\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{B851F137-2A1A-4D75-B183-34141935BEAB}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{221EA7DF-3087-4C6D-8D92-CB7F9E368ACA}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17430" windowHeight="10050" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -880,6 +880,45 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="9" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="18" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -931,47 +970,8 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="9" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="18" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1294,7 +1294,7 @@
   <dimension ref="A2:K4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1312,65 +1312,65 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:11" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="85" t="s">
+      <c r="A2" s="68" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="85" t="s">
+      <c r="B2" s="68" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="86" t="s">
+      <c r="C2" s="69" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="85" t="s">
+      <c r="D2" s="68" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="85" t="s">
+      <c r="E2" s="68" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="86" t="s">
+      <c r="F2" s="69" t="s">
         <v>27</v>
       </c>
-      <c r="G2" s="86" t="s">
+      <c r="G2" s="69" t="s">
         <v>26</v>
       </c>
-      <c r="H2" s="85" t="s">
+      <c r="H2" s="68" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="87" t="s">
+      <c r="I2" s="70" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="85" t="s">
+      <c r="J2" s="68" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="85" t="s">
+      <c r="K2" s="68" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="88"/>
-      <c r="B3" s="89"/>
-      <c r="C3" s="89"/>
-      <c r="D3" s="89"/>
-      <c r="E3" s="90"/>
-      <c r="F3" s="91"/>
-      <c r="G3" s="91"/>
-      <c r="H3" s="89"/>
-      <c r="I3" s="92"/>
-      <c r="J3" s="93"/>
-      <c r="K3" s="94"/>
+      <c r="A3" s="98"/>
+      <c r="B3" s="71"/>
+      <c r="C3" s="71"/>
+      <c r="D3" s="71"/>
+      <c r="E3" s="72"/>
+      <c r="F3" s="73"/>
+      <c r="G3" s="73"/>
+      <c r="H3" s="71"/>
+      <c r="I3" s="74"/>
+      <c r="J3" s="75"/>
+      <c r="K3" s="76"/>
     </row>
     <row r="4" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="95"/>
-      <c r="B4" s="95"/>
-      <c r="C4" s="95"/>
-      <c r="D4" s="95"/>
-      <c r="E4" s="96"/>
-      <c r="F4" s="97"/>
-      <c r="G4" s="97"/>
-      <c r="H4" s="95"/>
-      <c r="I4" s="98"/>
-      <c r="J4" s="98"/>
-      <c r="K4" s="98"/>
+      <c r="A4" s="77"/>
+      <c r="B4" s="77"/>
+      <c r="C4" s="77"/>
+      <c r="D4" s="77"/>
+      <c r="E4" s="78"/>
+      <c r="F4" s="79"/>
+      <c r="G4" s="79"/>
+      <c r="H4" s="77"/>
+      <c r="I4" s="80"/>
+      <c r="J4" s="80"/>
+      <c r="K4" s="80"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1464,7 +1464,7 @@
         <v>63</v>
       </c>
       <c r="I3" s="48"/>
-      <c r="J3" s="68" t="s">
+      <c r="J3" s="81" t="s">
         <v>44</v>
       </c>
       <c r="K3" s="52" t="s">
@@ -1497,7 +1497,7 @@
         <v>46</v>
       </c>
       <c r="I4" s="32"/>
-      <c r="J4" s="69"/>
+      <c r="J4" s="82"/>
       <c r="K4" s="52" t="s">
         <v>48</v>
       </c>
@@ -1528,7 +1528,7 @@
         <v>46</v>
       </c>
       <c r="I5" s="32"/>
-      <c r="J5" s="69"/>
+      <c r="J5" s="82"/>
       <c r="K5" s="52" t="s">
         <v>40</v>
       </c>
@@ -1559,7 +1559,7 @@
         <v>47</v>
       </c>
       <c r="I6" s="32"/>
-      <c r="J6" s="70"/>
+      <c r="J6" s="83"/>
       <c r="K6" s="52"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -1601,7 +1601,7 @@
         <v>64</v>
       </c>
       <c r="I8" s="32"/>
-      <c r="J8" s="68" t="s">
+      <c r="J8" s="81" t="s">
         <v>65</v>
       </c>
       <c r="K8" s="52" t="s">
@@ -1634,7 +1634,7 @@
         <v>46</v>
       </c>
       <c r="I9" s="32"/>
-      <c r="J9" s="69"/>
+      <c r="J9" s="82"/>
       <c r="K9" s="52" t="s">
         <v>50</v>
       </c>
@@ -1665,7 +1665,7 @@
         <v>46</v>
       </c>
       <c r="I10" s="32"/>
-      <c r="J10" s="69"/>
+      <c r="J10" s="82"/>
       <c r="K10" s="52"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -1707,7 +1707,7 @@
         <v>66</v>
       </c>
       <c r="I12" s="32"/>
-      <c r="J12" s="68"/>
+      <c r="J12" s="81"/>
       <c r="K12" s="52" t="s">
         <v>38</v>
       </c>
@@ -1740,7 +1740,7 @@
       <c r="I13" s="32">
         <v>42740</v>
       </c>
-      <c r="J13" s="69"/>
+      <c r="J13" s="82"/>
       <c r="K13" s="52" t="s">
         <v>50</v>
       </c>
@@ -1773,7 +1773,7 @@
       <c r="I14" s="32">
         <v>42740</v>
       </c>
-      <c r="J14" s="69"/>
+      <c r="J14" s="82"/>
       <c r="K14" s="52"/>
     </row>
     <row r="15" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -1804,7 +1804,7 @@
       <c r="I15" s="32">
         <v>42740</v>
       </c>
-      <c r="J15" s="69"/>
+      <c r="J15" s="82"/>
       <c r="K15" s="52"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -1848,7 +1848,7 @@
       <c r="I17" s="32">
         <v>43054</v>
       </c>
-      <c r="J17" s="68" t="s">
+      <c r="J17" s="81" t="s">
         <v>60</v>
       </c>
       <c r="K17" s="52" t="s">
@@ -1883,7 +1883,7 @@
       <c r="I18" s="32">
         <v>42738</v>
       </c>
-      <c r="J18" s="69"/>
+      <c r="J18" s="82"/>
       <c r="K18" s="52" t="s">
         <v>61</v>
       </c>
@@ -1916,7 +1916,7 @@
       <c r="I19" s="32">
         <v>42738</v>
       </c>
-      <c r="J19" s="69"/>
+      <c r="J19" s="82"/>
       <c r="K19" s="52" t="s">
         <v>62</v>
       </c>
@@ -1962,7 +1962,7 @@
       <c r="I21" s="32">
         <v>43049</v>
       </c>
-      <c r="J21" s="73"/>
+      <c r="J21" s="86"/>
       <c r="K21" s="52" t="s">
         <v>38</v>
       </c>
@@ -1995,7 +1995,7 @@
       <c r="I22" s="32">
         <v>43080</v>
       </c>
-      <c r="J22" s="74"/>
+      <c r="J22" s="87"/>
       <c r="K22" s="52" t="s">
         <v>61</v>
       </c>
@@ -2010,7 +2010,7 @@
       <c r="G23" s="47"/>
       <c r="H23" s="45"/>
       <c r="I23" s="32"/>
-      <c r="J23" s="75"/>
+      <c r="J23" s="88"/>
       <c r="K23" s="53" t="s">
         <v>73</v>
       </c>
@@ -2056,7 +2056,7 @@
       <c r="I25" s="32">
         <v>43049</v>
       </c>
-      <c r="J25" s="68"/>
+      <c r="J25" s="81"/>
       <c r="K25" s="52" t="s">
         <v>38</v>
       </c>
@@ -2089,7 +2089,7 @@
       <c r="I26" s="32">
         <v>43090</v>
       </c>
-      <c r="J26" s="69"/>
+      <c r="J26" s="82"/>
       <c r="K26" s="52" t="s">
         <v>72</v>
       </c>
@@ -2135,7 +2135,7 @@
       <c r="I28" s="32">
         <v>43049</v>
       </c>
-      <c r="J28" s="71" t="s">
+      <c r="J28" s="84" t="s">
         <v>85</v>
       </c>
       <c r="K28" s="52" t="s">
@@ -2170,7 +2170,7 @@
       <c r="I29" s="32">
         <v>43049</v>
       </c>
-      <c r="J29" s="72"/>
+      <c r="J29" s="85"/>
       <c r="K29" s="52" t="s">
         <v>78</v>
       </c>
@@ -2203,7 +2203,7 @@
       <c r="I30" s="32">
         <v>43049</v>
       </c>
-      <c r="J30" s="72"/>
+      <c r="J30" s="85"/>
       <c r="K30" s="52"/>
     </row>
     <row r="31" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -2234,7 +2234,7 @@
       <c r="I31" s="49">
         <v>43063</v>
       </c>
-      <c r="J31" s="72"/>
+      <c r="J31" s="85"/>
       <c r="K31" s="52"/>
     </row>
     <row r="44" spans="1:11" ht="51" x14ac:dyDescent="0.25">
@@ -2408,10 +2408,10 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="76" t="s">
+      <c r="A3" s="89" t="s">
         <v>41</v>
       </c>
-      <c r="B3" s="76" t="s">
+      <c r="B3" s="89" t="s">
         <v>24</v>
       </c>
       <c r="C3" s="8">
@@ -2432,13 +2432,13 @@
       <c r="H3" s="12">
         <v>43081</v>
       </c>
-      <c r="I3" s="77" t="s">
+      <c r="I3" s="90" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="76"/>
-      <c r="B4" s="76"/>
+      <c r="A4" s="89"/>
+      <c r="B4" s="89"/>
       <c r="C4" s="8" t="s">
         <v>10</v>
       </c>
@@ -2455,13 +2455,13 @@
         <v>12</v>
       </c>
       <c r="H4" s="8"/>
-      <c r="I4" s="77"/>
+      <c r="I4" s="90"/>
     </row>
     <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="78" t="s">
+      <c r="A5" s="91" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="78"/>
+      <c r="B5" s="91"/>
       <c r="C5" s="8" t="s">
         <v>14</v>
       </c>
@@ -2478,13 +2478,13 @@
         <v>12</v>
       </c>
       <c r="H5" s="8"/>
-      <c r="I5" s="77"/>
+      <c r="I5" s="90"/>
     </row>
     <row r="6" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="79" t="s">
+      <c r="A6" s="92" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="79"/>
+      <c r="B6" s="92"/>
       <c r="C6" s="8">
         <v>1</v>
       </c>
@@ -2503,7 +2503,7 @@
       <c r="H6" s="6">
         <v>43081</v>
       </c>
-      <c r="I6" s="77"/>
+      <c r="I6" s="90"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C7" s="34">
@@ -2524,7 +2524,7 @@
       <c r="H7" s="6">
         <v>43087</v>
       </c>
-      <c r="I7" s="77"/>
+      <c r="I7" s="90"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C11" s="1"/>
@@ -2597,10 +2597,10 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="76" t="s">
+      <c r="A3" s="89" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="76" t="s">
+      <c r="B3" s="89" t="s">
         <v>24</v>
       </c>
       <c r="C3" s="8">
@@ -2621,13 +2621,13 @@
       <c r="H3" s="12">
         <v>43081</v>
       </c>
-      <c r="I3" s="77" t="s">
+      <c r="I3" s="90" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="76"/>
-      <c r="B4" s="76"/>
+      <c r="A4" s="89"/>
+      <c r="B4" s="89"/>
       <c r="C4" s="8" t="s">
         <v>10</v>
       </c>
@@ -2644,13 +2644,13 @@
         <v>12</v>
       </c>
       <c r="H4" s="7"/>
-      <c r="I4" s="77"/>
+      <c r="I4" s="90"/>
     </row>
     <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="78" t="s">
+      <c r="A5" s="91" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="78"/>
+      <c r="B5" s="91"/>
       <c r="C5" s="8" t="s">
         <v>14</v>
       </c>
@@ -2667,13 +2667,13 @@
         <v>12</v>
       </c>
       <c r="H5" s="7"/>
-      <c r="I5" s="77"/>
+      <c r="I5" s="90"/>
     </row>
     <row r="6" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="79" t="s">
+      <c r="A6" s="92" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="79"/>
+      <c r="B6" s="92"/>
       <c r="C6" s="8">
         <v>1</v>
       </c>
@@ -2692,7 +2692,7 @@
       <c r="H6" s="6">
         <v>43081</v>
       </c>
-      <c r="I6" s="77"/>
+      <c r="I6" s="90"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C7" s="34">
@@ -2713,7 +2713,7 @@
       <c r="H7" s="6">
         <v>43087</v>
       </c>
-      <c r="I7" s="77"/>
+      <c r="I7" s="90"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C11" s="1"/>
@@ -2786,13 +2786,13 @@
       </c>
     </row>
     <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="76" t="s">
+      <c r="A4" s="89" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="C4" s="80"/>
+      <c r="C4" s="93"/>
       <c r="D4" s="31" t="s">
         <v>26</v>
       </c>
@@ -2813,11 +2813,11 @@
       </c>
     </row>
     <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="76"/>
+      <c r="A5" s="89"/>
       <c r="B5" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="80"/>
+      <c r="C5" s="93"/>
       <c r="D5" s="31" t="s">
         <v>27</v>
       </c>
@@ -2838,11 +2838,11 @@
       </c>
     </row>
     <row r="6" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="76"/>
+      <c r="A6" s="89"/>
       <c r="B6" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="C6" s="80"/>
+      <c r="C6" s="93"/>
       <c r="D6" s="31" t="s">
         <v>6</v>
       </c>
@@ -2863,9 +2863,9 @@
       </c>
     </row>
     <row r="7" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="76"/>
+      <c r="A7" s="89"/>
       <c r="B7" s="33"/>
-      <c r="C7" s="80"/>
+      <c r="C7" s="93"/>
       <c r="D7" s="31" t="s">
         <v>7</v>
       </c>
@@ -2917,7 +2917,7 @@
       <c r="L9" s="67"/>
     </row>
     <row r="10" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="76" t="s">
+      <c r="A10" s="89" t="s">
         <v>2</v>
       </c>
       <c r="B10" s="33" t="s">
@@ -2936,10 +2936,10 @@
       <c r="G10" s="22">
         <v>20</v>
       </c>
-      <c r="H10" s="80"/>
+      <c r="H10" s="93"/>
     </row>
     <row r="11" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="76"/>
+      <c r="A11" s="89"/>
       <c r="B11" s="33" t="s">
         <v>39</v>
       </c>
@@ -2956,10 +2956,10 @@
       <c r="G11" s="22">
         <v>20</v>
       </c>
-      <c r="H11" s="80"/>
+      <c r="H11" s="93"/>
     </row>
     <row r="12" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="76"/>
+      <c r="A12" s="89"/>
       <c r="B12" s="33" t="s">
         <v>40</v>
       </c>
@@ -2976,10 +2976,10 @@
       <c r="G12" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="H12" s="80"/>
+      <c r="H12" s="93"/>
     </row>
     <row r="13" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="76"/>
+      <c r="A13" s="89"/>
       <c r="B13" s="33"/>
       <c r="C13" s="31"/>
       <c r="D13" s="31" t="s">
@@ -2990,7 +2990,7 @@
       </c>
       <c r="F13" s="22"/>
       <c r="G13" s="22"/>
-      <c r="H13" s="80"/>
+      <c r="H13" s="93"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -3034,15 +3034,15 @@
       <c r="A4" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="81" t="s">
+      <c r="B4" s="94" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="81"/>
-      <c r="D4" s="81"/>
-      <c r="E4" s="81" t="s">
+      <c r="C4" s="94"/>
+      <c r="D4" s="94"/>
+      <c r="E4" s="94" t="s">
         <v>20</v>
       </c>
-      <c r="F4" s="81"/>
+      <c r="F4" s="94"/>
       <c r="G4" s="29" t="s">
         <v>21</v>
       </c>
@@ -3051,16 +3051,16 @@
       <c r="A5" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="82"/>
-      <c r="C5" s="82"/>
-      <c r="D5" s="82"/>
+      <c r="B5" s="95"/>
+      <c r="C5" s="95"/>
+      <c r="D5" s="95"/>
       <c r="E5" s="29" t="s">
         <v>22</v>
       </c>
       <c r="F5" s="26">
         <v>43081</v>
       </c>
-      <c r="G5" s="83" t="s">
+      <c r="G5" s="96" t="s">
         <v>23</v>
       </c>
     </row>
@@ -3068,31 +3068,31 @@
       <c r="A6" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="82"/>
-      <c r="C6" s="82"/>
-      <c r="D6" s="82"/>
+      <c r="B6" s="95"/>
+      <c r="C6" s="95"/>
+      <c r="D6" s="95"/>
       <c r="E6" s="29" t="s">
         <v>5</v>
       </c>
       <c r="F6" s="27">
         <v>24</v>
       </c>
-      <c r="G6" s="83"/>
+      <c r="G6" s="96"/>
     </row>
     <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="82"/>
-      <c r="C7" s="82"/>
-      <c r="D7" s="82"/>
+      <c r="B7" s="95"/>
+      <c r="C7" s="95"/>
+      <c r="D7" s="95"/>
       <c r="E7" s="29" t="s">
         <v>25</v>
       </c>
       <c r="F7" s="26">
         <v>43079</v>
       </c>
-      <c r="G7" s="83"/>
+      <c r="G7" s="96"/>
     </row>
     <row r="8" spans="1:7" ht="7.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="18"/>
@@ -3143,7 +3143,7 @@
         <v>12</v>
       </c>
       <c r="F10" s="22"/>
-      <c r="G10" s="84" t="s">
+      <c r="G10" s="97" t="s">
         <v>28</v>
       </c>
     </row>
@@ -3164,7 +3164,7 @@
         <v>12</v>
       </c>
       <c r="F11" s="22"/>
-      <c r="G11" s="84"/>
+      <c r="G11" s="97"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="22">
@@ -3185,7 +3185,7 @@
       <c r="F12" s="24">
         <v>43081</v>
       </c>
-      <c r="G12" s="84"/>
+      <c r="G12" s="97"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="22">
@@ -3206,21 +3206,21 @@
       <c r="F13" s="24">
         <v>43087</v>
       </c>
-      <c r="G13" s="84"/>
+      <c r="G13" s="97"/>
     </row>
     <row r="15" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B15" s="78" t="s">
+      <c r="B15" s="91" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="78"/>
-      <c r="D15" s="78"/>
-      <c r="E15" s="78" t="s">
+      <c r="C15" s="91"/>
+      <c r="D15" s="91"/>
+      <c r="E15" s="91" t="s">
         <v>20</v>
       </c>
-      <c r="F15" s="78"/>
+      <c r="F15" s="91"/>
       <c r="G15" s="14" t="s">
         <v>21</v>
       </c>
@@ -3229,16 +3229,16 @@
       <c r="A16" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B16" s="79"/>
-      <c r="C16" s="79"/>
-      <c r="D16" s="79"/>
+      <c r="B16" s="92"/>
+      <c r="C16" s="92"/>
+      <c r="D16" s="92"/>
       <c r="E16" s="14" t="s">
         <v>22</v>
       </c>
       <c r="F16" s="16">
         <v>43081</v>
       </c>
-      <c r="G16" s="76" t="s">
+      <c r="G16" s="89" t="s">
         <v>23</v>
       </c>
     </row>
@@ -3246,31 +3246,31 @@
       <c r="A17" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="79"/>
-      <c r="C17" s="79"/>
-      <c r="D17" s="79"/>
+      <c r="B17" s="92"/>
+      <c r="C17" s="92"/>
+      <c r="D17" s="92"/>
       <c r="E17" s="14" t="s">
         <v>5</v>
       </c>
       <c r="F17" s="17">
         <v>24</v>
       </c>
-      <c r="G17" s="76"/>
+      <c r="G17" s="89"/>
     </row>
     <row r="18" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="B18" s="79"/>
-      <c r="C18" s="79"/>
-      <c r="D18" s="79"/>
+      <c r="B18" s="92"/>
+      <c r="C18" s="92"/>
+      <c r="D18" s="92"/>
       <c r="E18" s="14" t="s">
         <v>25</v>
       </c>
       <c r="F18" s="16">
         <v>43079</v>
       </c>
-      <c r="G18" s="76"/>
+      <c r="G18" s="89"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
@@ -3312,7 +3312,7 @@
         <v>12</v>
       </c>
       <c r="F21" s="7"/>
-      <c r="G21" s="77" t="s">
+      <c r="G21" s="90" t="s">
         <v>28</v>
       </c>
     </row>
@@ -3333,7 +3333,7 @@
         <v>12</v>
       </c>
       <c r="F22" s="7"/>
-      <c r="G22" s="77"/>
+      <c r="G22" s="90"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="7">
@@ -3354,7 +3354,7 @@
       <c r="F23" s="6">
         <v>43081</v>
       </c>
-      <c r="G23" s="77"/>
+      <c r="G23" s="90"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="7">
@@ -3375,7 +3375,7 @@
       <c r="F24" s="6">
         <v>43087</v>
       </c>
-      <c r="G24" s="77"/>
+      <c r="G24" s="90"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -3396,12 +3396,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005385EB61B379B64FA3FA00EFD5F48211" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="15b97f2a5ef9ff731d6c6b6a53c29c79">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8fb9fcf7-a6bd-4cda-a801-5717a79e1e97" xmlns:ns3="b1338d7f-541f-4bc8-84bc-74292fa164fd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bdf937eed7c5c26b74985f5c8ee9608f" ns2:_="" ns3:_="">
     <xsd:import namespace="8fb9fcf7-a6bd-4cda-a801-5717a79e1e97"/>
@@ -3566,6 +3560,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -3576,23 +3576,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5C94C584-4AAB-4B64-8188-315FD51E3EE4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="b1338d7f-541f-4bc8-84bc-74292fa164fd"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="8fb9fcf7-a6bd-4cda-a801-5717a79e1e97"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{87464A97-8BFD-499C-AE46-83C4EA3F84BB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3611,6 +3594,23 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5C94C584-4AAB-4B64-8188-315FD51E3EE4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="b1338d7f-541f-4bc8-84bc-74292fa164fd"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="8fb9fcf7-a6bd-4cda-a801-5717a79e1e97"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E2473AE6-58EA-4483-BA75-FF2FBA4C0E2B}">
   <ds:schemaRefs>

</xml_diff>